<commit_message>
separacao de responsabilidade: logica.py dividido
</commit_message>
<xml_diff>
--- a/relatorios/relatorio_frequencia_231025.xlsx
+++ b/relatorios/relatorio_frequencia_231025.xlsx
@@ -80,7 +80,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -94,46 +94,17 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -523,79 +494,82 @@
           <t>Relatório de Frequência - Quinta-feira, 23/10/2025</t>
         </is>
       </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="2" t="n"/>
     </row>
     <row r="2"/>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>TURMA: EF1601</t>
         </is>
       </c>
-      <c r="B3" s="3" t="n"/>
-      <c r="C3" s="3" t="n"/>
-      <c r="D3" s="4" t="n"/>
+      <c r="B3" s="2" t="n"/>
+      <c r="C3" s="2" t="n"/>
+      <c r="D3" s="2" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="inlineStr">
+      <c r="A4" s="4" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B4" s="5" t="inlineStr">
+      <c r="B4" s="4" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C4" s="5" t="inlineStr">
+      <c r="C4" s="4" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D4" s="5" t="inlineStr">
+      <c r="D4" s="4" t="inlineStr">
         <is>
           <t>Acesso</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="inlineStr">
+      <c r="A5" s="5" t="inlineStr">
         <is>
           <t>2944001118</t>
         </is>
       </c>
-      <c r="B5" s="6" t="inlineStr">
+      <c r="B5" s="5" t="inlineStr">
         <is>
           <t>Eric Marques Garcia</t>
         </is>
       </c>
-      <c r="C5" s="6" t="inlineStr">
+      <c r="C5" s="5" t="inlineStr">
         <is>
           <t>SAIU CEDO</t>
         </is>
       </c>
-      <c r="D5" s="6" t="inlineStr">
+      <c r="D5" s="5" t="inlineStr">
         <is>
           <t>Saída: 08:48:23</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="7" t="inlineStr">
+      <c r="A6" s="6" t="inlineStr">
         <is>
           <t>2025000741</t>
         </is>
       </c>
-      <c r="B6" s="7" t="inlineStr">
+      <c r="B6" s="6" t="inlineStr">
         <is>
           <t>Mel Glória Nogueira Medeiros</t>
         </is>
       </c>
-      <c r="C6" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D6" s="7" t="inlineStr">
+      <c r="C6" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D6" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
@@ -603,54 +577,54 @@
     </row>
     <row r="7"/>
     <row r="8">
-      <c r="A8" s="2" t="inlineStr">
+      <c r="A8" s="3" t="inlineStr">
         <is>
           <t>TURMA: EF1602</t>
         </is>
       </c>
-      <c r="B8" s="3" t="n"/>
-      <c r="C8" s="3" t="n"/>
-      <c r="D8" s="4" t="n"/>
+      <c r="B8" s="2" t="n"/>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="inlineStr">
+      <c r="A9" s="4" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B9" s="5" t="inlineStr">
+      <c r="B9" s="4" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C9" s="5" t="inlineStr">
+      <c r="C9" s="4" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D9" s="5" t="inlineStr">
+      <c r="D9" s="4" t="inlineStr">
         <is>
           <t>Acesso</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="7" t="inlineStr">
+      <c r="A10" s="6" t="inlineStr">
         <is>
           <t>2022321442</t>
         </is>
       </c>
-      <c r="B10" s="7" t="inlineStr">
+      <c r="B10" s="6" t="inlineStr">
         <is>
           <t>Ana Clara Draxler dos Reis de Souza</t>
         </is>
       </c>
-      <c r="C10" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D10" s="7" t="inlineStr">
+      <c r="C10" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D10" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
@@ -658,76 +632,76 @@
     </row>
     <row r="11"/>
     <row r="12">
-      <c r="A12" s="2" t="inlineStr">
+      <c r="A12" s="3" t="inlineStr">
         <is>
           <t>TURMA: EF1701</t>
         </is>
       </c>
-      <c r="B12" s="3" t="n"/>
-      <c r="C12" s="3" t="n"/>
-      <c r="D12" s="4" t="n"/>
+      <c r="B12" s="2" t="n"/>
+      <c r="C12" s="2" t="n"/>
+      <c r="D12" s="2" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="inlineStr">
+      <c r="A13" s="4" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B13" s="5" t="inlineStr">
+      <c r="B13" s="4" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C13" s="5" t="inlineStr">
+      <c r="C13" s="4" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D13" s="5" t="inlineStr">
+      <c r="D13" s="4" t="inlineStr">
         <is>
           <t>Acesso</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="7" t="inlineStr">
+      <c r="A14" s="6" t="inlineStr">
         <is>
           <t>2022321462</t>
         </is>
       </c>
-      <c r="B14" s="7" t="inlineStr">
+      <c r="B14" s="6" t="inlineStr">
         <is>
           <t>Alice Ferreira Oliveira da Silva</t>
         </is>
       </c>
-      <c r="C14" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D14" s="7" t="inlineStr">
+      <c r="C14" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D14" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="7" t="inlineStr">
+      <c r="A15" s="6" t="inlineStr">
         <is>
           <t>2024000415</t>
         </is>
       </c>
-      <c r="B15" s="7" t="inlineStr">
+      <c r="B15" s="6" t="inlineStr">
         <is>
           <t>Isis Almenara Bitencourt</t>
         </is>
       </c>
-      <c r="C15" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D15" s="7" t="inlineStr">
+      <c r="C15" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D15" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
@@ -735,120 +709,120 @@
     </row>
     <row r="16"/>
     <row r="17">
-      <c r="A17" s="2" t="inlineStr">
+      <c r="A17" s="3" t="inlineStr">
         <is>
           <t>TURMA: EF1702</t>
         </is>
       </c>
-      <c r="B17" s="3" t="n"/>
-      <c r="C17" s="3" t="n"/>
-      <c r="D17" s="4" t="n"/>
+      <c r="B17" s="2" t="n"/>
+      <c r="C17" s="2" t="n"/>
+      <c r="D17" s="2" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="5" t="inlineStr">
+      <c r="A18" s="4" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B18" s="5" t="inlineStr">
+      <c r="B18" s="4" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C18" s="5" t="inlineStr">
+      <c r="C18" s="4" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D18" s="5" t="inlineStr">
+      <c r="D18" s="4" t="inlineStr">
         <is>
           <t>Acesso</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="6" t="inlineStr">
+      <c r="A19" s="5" t="inlineStr">
         <is>
           <t>2024000420</t>
         </is>
       </c>
-      <c r="B19" s="6" t="inlineStr">
+      <c r="B19" s="5" t="inlineStr">
         <is>
           <t>Ana Luísa Pecly do Prado</t>
         </is>
       </c>
-      <c r="C19" s="6" t="inlineStr">
+      <c r="C19" s="5" t="inlineStr">
         <is>
           <t>SAIU CEDO</t>
         </is>
       </c>
-      <c r="D19" s="6" t="inlineStr">
+      <c r="D19" s="5" t="inlineStr">
         <is>
           <t>Saída: 10:59:02</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="6" t="inlineStr">
+      <c r="A20" s="5" t="inlineStr">
         <is>
           <t>2024000422</t>
         </is>
       </c>
-      <c r="B20" s="6" t="inlineStr">
+      <c r="B20" s="5" t="inlineStr">
         <is>
           <t>Antenor Satolo Cucco</t>
         </is>
       </c>
-      <c r="C20" s="6" t="inlineStr">
+      <c r="C20" s="5" t="inlineStr">
         <is>
           <t>SAIU CEDO</t>
         </is>
       </c>
-      <c r="D20" s="6" t="inlineStr">
+      <c r="D20" s="5" t="inlineStr">
         <is>
           <t>Saída: 10:59:52</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="6" t="inlineStr">
+      <c r="A21" s="5" t="inlineStr">
         <is>
           <t>2022321011</t>
         </is>
       </c>
-      <c r="B21" s="6" t="inlineStr">
+      <c r="B21" s="5" t="inlineStr">
         <is>
           <t>Louise Roli Terra</t>
         </is>
       </c>
-      <c r="C21" s="6" t="inlineStr">
+      <c r="C21" s="5" t="inlineStr">
         <is>
           <t>SAIU CEDO</t>
         </is>
       </c>
-      <c r="D21" s="6" t="inlineStr">
+      <c r="D21" s="5" t="inlineStr">
         <is>
           <t>Saída: 11:19:30</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="8" t="inlineStr">
+      <c r="A22" s="7" t="inlineStr">
         <is>
           <t>2022321429</t>
         </is>
       </c>
-      <c r="B22" s="8" t="inlineStr">
+      <c r="B22" s="7" t="inlineStr">
         <is>
           <t>Luna Trócilo Rodrigues Lopes</t>
         </is>
       </c>
-      <c r="C22" s="8" t="inlineStr">
+      <c r="C22" s="7" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D22" s="8" t="inlineStr">
+      <c r="D22" s="7" t="inlineStr">
         <is>
           <t>Entrada: 08:53:41</t>
         </is>
@@ -856,98 +830,98 @@
     </row>
     <row r="23"/>
     <row r="24">
-      <c r="A24" s="2" t="inlineStr">
+      <c r="A24" s="3" t="inlineStr">
         <is>
           <t>TURMA: EF1801</t>
         </is>
       </c>
-      <c r="B24" s="3" t="n"/>
-      <c r="C24" s="3" t="n"/>
-      <c r="D24" s="4" t="n"/>
+      <c r="B24" s="2" t="n"/>
+      <c r="C24" s="2" t="n"/>
+      <c r="D24" s="2" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="5" t="inlineStr">
+      <c r="A25" s="4" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B25" s="5" t="inlineStr">
+      <c r="B25" s="4" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C25" s="5" t="inlineStr">
+      <c r="C25" s="4" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D25" s="5" t="inlineStr">
+      <c r="D25" s="4" t="inlineStr">
         <is>
           <t>Acesso</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="8" t="inlineStr">
+      <c r="A26" s="7" t="inlineStr">
         <is>
           <t>2370001115</t>
         </is>
       </c>
-      <c r="B26" s="8" t="inlineStr">
+      <c r="B26" s="7" t="inlineStr">
         <is>
           <t>Benício Cabelino Rabelo</t>
         </is>
       </c>
-      <c r="C26" s="8" t="inlineStr">
+      <c r="C26" s="7" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D26" s="8" t="inlineStr">
+      <c r="D26" s="7" t="inlineStr">
         <is>
           <t>Entrada: 08:47:00</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="8" t="inlineStr">
+      <c r="A27" s="7" t="inlineStr">
         <is>
           <t>2171001114</t>
         </is>
       </c>
-      <c r="B27" s="8" t="inlineStr">
+      <c r="B27" s="7" t="inlineStr">
         <is>
           <t>Maria Fernanda Ramires Zampier</t>
         </is>
       </c>
-      <c r="C27" s="8" t="inlineStr">
+      <c r="C27" s="7" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D27" s="8" t="inlineStr">
+      <c r="D27" s="7" t="inlineStr">
         <is>
           <t>Entrada: 08:47:05</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="7" t="inlineStr">
+      <c r="A28" s="6" t="inlineStr">
         <is>
           <t>2768001117</t>
         </is>
       </c>
-      <c r="B28" s="7" t="inlineStr">
+      <c r="B28" s="6" t="inlineStr">
         <is>
           <t>Matheus Jazom Almeida Gonçalves</t>
         </is>
       </c>
-      <c r="C28" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D28" s="7" t="inlineStr">
+      <c r="C28" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D28" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
@@ -955,120 +929,120 @@
     </row>
     <row r="29"/>
     <row r="30">
-      <c r="A30" s="2" t="inlineStr">
+      <c r="A30" s="3" t="inlineStr">
         <is>
           <t>TURMA: EF1803</t>
         </is>
       </c>
-      <c r="B30" s="3" t="n"/>
-      <c r="C30" s="3" t="n"/>
-      <c r="D30" s="4" t="n"/>
+      <c r="B30" s="2" t="n"/>
+      <c r="C30" s="2" t="n"/>
+      <c r="D30" s="2" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="5" t="inlineStr">
+      <c r="A31" s="4" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B31" s="5" t="inlineStr">
+      <c r="B31" s="4" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C31" s="5" t="inlineStr">
+      <c r="C31" s="4" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D31" s="5" t="inlineStr">
+      <c r="D31" s="4" t="inlineStr">
         <is>
           <t>Acesso</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="7" t="inlineStr">
+      <c r="A32" s="6" t="inlineStr">
         <is>
           <t>2024000516</t>
         </is>
       </c>
-      <c r="B32" s="7" t="inlineStr">
+      <c r="B32" s="6" t="inlineStr">
         <is>
           <t>João Gabriel Levoni Carvalho</t>
         </is>
       </c>
-      <c r="C32" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D32" s="7" t="inlineStr">
+      <c r="C32" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D32" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="6" t="inlineStr">
+      <c r="A33" s="5" t="inlineStr">
         <is>
           <t>2022016100</t>
         </is>
       </c>
-      <c r="B33" s="6" t="inlineStr">
+      <c r="B33" s="5" t="inlineStr">
         <is>
           <t>Luisa Guimarães Boechat</t>
         </is>
       </c>
-      <c r="C33" s="6" t="inlineStr">
+      <c r="C33" s="5" t="inlineStr">
         <is>
           <t>SAIU CEDO</t>
         </is>
       </c>
-      <c r="D33" s="6" t="inlineStr">
+      <c r="D33" s="5" t="inlineStr">
         <is>
           <t>Saída: 08:23:59</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="6" t="inlineStr">
+      <c r="A34" s="5" t="inlineStr">
         <is>
           <t>2022016200</t>
         </is>
       </c>
-      <c r="B34" s="6" t="inlineStr">
+      <c r="B34" s="5" t="inlineStr">
         <is>
           <t>Matheus de Souza Lannes</t>
         </is>
       </c>
-      <c r="C34" s="6" t="inlineStr">
+      <c r="C34" s="5" t="inlineStr">
         <is>
           <t>SAIU CEDO</t>
         </is>
       </c>
-      <c r="D34" s="6" t="inlineStr">
+      <c r="D34" s="5" t="inlineStr">
         <is>
           <t>Saída: 10:14:16</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="6" t="inlineStr">
+      <c r="A35" s="5" t="inlineStr">
         <is>
           <t>2025000750</t>
         </is>
       </c>
-      <c r="B35" s="6" t="inlineStr">
+      <c r="B35" s="5" t="inlineStr">
         <is>
           <t>Rafael Cordeiro Ferreira</t>
         </is>
       </c>
-      <c r="C35" s="6" t="inlineStr">
+      <c r="C35" s="5" t="inlineStr">
         <is>
           <t>SAIU CEDO</t>
         </is>
       </c>
-      <c r="D35" s="6" t="inlineStr">
+      <c r="D35" s="5" t="inlineStr">
         <is>
           <t>Saída: 08:22:58</t>
         </is>
@@ -1076,76 +1050,76 @@
     </row>
     <row r="36"/>
     <row r="37">
-      <c r="A37" s="2" t="inlineStr">
+      <c r="A37" s="3" t="inlineStr">
         <is>
           <t>TURMA: EF1901</t>
         </is>
       </c>
-      <c r="B37" s="3" t="n"/>
-      <c r="C37" s="3" t="n"/>
-      <c r="D37" s="4" t="n"/>
+      <c r="B37" s="2" t="n"/>
+      <c r="C37" s="2" t="n"/>
+      <c r="D37" s="2" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="5" t="inlineStr">
+      <c r="A38" s="4" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B38" s="5" t="inlineStr">
+      <c r="B38" s="4" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C38" s="5" t="inlineStr">
+      <c r="C38" s="4" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D38" s="5" t="inlineStr">
+      <c r="D38" s="4" t="inlineStr">
         <is>
           <t>Acesso</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="7" t="inlineStr">
+      <c r="A39" s="6" t="inlineStr">
         <is>
           <t>3384001121</t>
         </is>
       </c>
-      <c r="B39" s="7" t="inlineStr">
+      <c r="B39" s="6" t="inlineStr">
         <is>
           <t>Antônio Marinho Calado</t>
         </is>
       </c>
-      <c r="C39" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D39" s="7" t="inlineStr">
+      <c r="C39" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D39" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="6" t="inlineStr">
+      <c r="A40" s="5" t="inlineStr">
         <is>
           <t>2025000705</t>
         </is>
       </c>
-      <c r="B40" s="6" t="inlineStr">
+      <c r="B40" s="5" t="inlineStr">
         <is>
           <t>Sarah Emunah Alves Tavares</t>
         </is>
       </c>
-      <c r="C40" s="6" t="inlineStr">
+      <c r="C40" s="5" t="inlineStr">
         <is>
           <t>SAIU CEDO</t>
         </is>
       </c>
-      <c r="D40" s="6" t="inlineStr">
+      <c r="D40" s="5" t="inlineStr">
         <is>
           <t>Saída: 11:14:57</t>
         </is>
@@ -1153,120 +1127,120 @@
     </row>
     <row r="41"/>
     <row r="42">
-      <c r="A42" s="2" t="inlineStr">
+      <c r="A42" s="3" t="inlineStr">
         <is>
           <t>TURMA: EF1902</t>
         </is>
       </c>
-      <c r="B42" s="3" t="n"/>
-      <c r="C42" s="3" t="n"/>
-      <c r="D42" s="4" t="n"/>
+      <c r="B42" s="2" t="n"/>
+      <c r="C42" s="2" t="n"/>
+      <c r="D42" s="2" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="5" t="inlineStr">
+      <c r="A43" s="4" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B43" s="5" t="inlineStr">
+      <c r="B43" s="4" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C43" s="5" t="inlineStr">
+      <c r="C43" s="4" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D43" s="5" t="inlineStr">
+      <c r="D43" s="4" t="inlineStr">
         <is>
           <t>Acesso</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="7" t="inlineStr">
+      <c r="A44" s="6" t="inlineStr">
         <is>
           <t>3665001122</t>
         </is>
       </c>
-      <c r="B44" s="7" t="inlineStr">
+      <c r="B44" s="6" t="inlineStr">
         <is>
           <t>Gabriel Carvalho Avelino</t>
         </is>
       </c>
-      <c r="C44" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D44" s="7" t="inlineStr">
+      <c r="C44" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D44" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="7" t="inlineStr">
+      <c r="A45" s="6" t="inlineStr">
         <is>
           <t>2025000709</t>
         </is>
       </c>
-      <c r="B45" s="7" t="inlineStr">
+      <c r="B45" s="6" t="inlineStr">
         <is>
           <t>Maria Eduarda Faria de Souza</t>
         </is>
       </c>
-      <c r="C45" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D45" s="7" t="inlineStr">
+      <c r="C45" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D45" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="6" t="inlineStr">
+      <c r="A46" s="5" t="inlineStr">
         <is>
           <t>2732001117</t>
         </is>
       </c>
-      <c r="B46" s="6" t="inlineStr">
+      <c r="B46" s="5" t="inlineStr">
         <is>
           <t>Miguel José Caldararo</t>
         </is>
       </c>
-      <c r="C46" s="6" t="inlineStr">
+      <c r="C46" s="5" t="inlineStr">
         <is>
           <t>SAIU CEDO</t>
         </is>
       </c>
-      <c r="D46" s="6" t="inlineStr">
+      <c r="D46" s="5" t="inlineStr">
         <is>
           <t>Saída: 08:27:42</t>
         </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="7" t="inlineStr">
+      <c r="A47" s="6" t="inlineStr">
         <is>
           <t>2025000743</t>
         </is>
       </c>
-      <c r="B47" s="7" t="inlineStr">
+      <c r="B47" s="6" t="inlineStr">
         <is>
           <t>Álvaro Souza Campos</t>
         </is>
       </c>
-      <c r="C47" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D47" s="7" t="inlineStr">
+      <c r="C47" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D47" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
@@ -1274,142 +1248,142 @@
     </row>
     <row r="48"/>
     <row r="49">
-      <c r="A49" s="2" t="inlineStr">
+      <c r="A49" s="3" t="inlineStr">
         <is>
           <t>TURMA: EM2101</t>
         </is>
       </c>
-      <c r="B49" s="3" t="n"/>
-      <c r="C49" s="3" t="n"/>
-      <c r="D49" s="4" t="n"/>
+      <c r="B49" s="2" t="n"/>
+      <c r="C49" s="2" t="n"/>
+      <c r="D49" s="2" t="n"/>
     </row>
     <row r="50">
-      <c r="A50" s="5" t="inlineStr">
+      <c r="A50" s="4" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B50" s="5" t="inlineStr">
+      <c r="B50" s="4" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C50" s="5" t="inlineStr">
+      <c r="C50" s="4" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D50" s="5" t="inlineStr">
+      <c r="D50" s="4" t="inlineStr">
         <is>
           <t>Acesso</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="8" t="inlineStr">
+      <c r="A51" s="7" t="inlineStr">
         <is>
           <t>2025000721</t>
         </is>
       </c>
-      <c r="B51" s="8" t="inlineStr">
+      <c r="B51" s="7" t="inlineStr">
         <is>
           <t>Bia Bastos Sueth</t>
         </is>
       </c>
-      <c r="C51" s="8" t="inlineStr">
+      <c r="C51" s="7" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D51" s="8" t="inlineStr">
+      <c r="D51" s="7" t="inlineStr">
         <is>
           <t>Entrada: 08:57:30</t>
         </is>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="7" t="inlineStr">
+      <c r="A52" s="6" t="inlineStr">
         <is>
           <t>2025000723</t>
         </is>
       </c>
-      <c r="B52" s="7" t="inlineStr">
+      <c r="B52" s="6" t="inlineStr">
         <is>
           <t>Felipe Côrte Real Tucher</t>
         </is>
       </c>
-      <c r="C52" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D52" s="7" t="inlineStr">
+      <c r="C52" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D52" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="8" t="inlineStr">
+      <c r="A53" s="7" t="inlineStr">
         <is>
           <t>2025000590</t>
         </is>
       </c>
-      <c r="B53" s="8" t="inlineStr">
+      <c r="B53" s="7" t="inlineStr">
         <is>
           <t>Laura Oliveira Barros da Silva</t>
         </is>
       </c>
-      <c r="C53" s="8" t="inlineStr">
+      <c r="C53" s="7" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D53" s="8" t="inlineStr">
+      <c r="D53" s="7" t="inlineStr">
         <is>
           <t>Entrada: 08:39:02</t>
         </is>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="8" t="inlineStr">
+      <c r="A54" s="7" t="inlineStr">
         <is>
           <t>2025000573</t>
         </is>
       </c>
-      <c r="B54" s="8" t="inlineStr">
+      <c r="B54" s="7" t="inlineStr">
         <is>
           <t>Luma de Oliveira Carvalho</t>
         </is>
       </c>
-      <c r="C54" s="8" t="inlineStr">
+      <c r="C54" s="7" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D54" s="8" t="inlineStr">
+      <c r="D54" s="7" t="inlineStr">
         <is>
           <t>Entrada: 08:46:22</t>
         </is>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="8" t="inlineStr">
+      <c r="A55" s="7" t="inlineStr">
         <is>
           <t>2025000579</t>
         </is>
       </c>
-      <c r="B55" s="8" t="inlineStr">
+      <c r="B55" s="7" t="inlineStr">
         <is>
           <t>Maria Luísa Gaudard Cardoso</t>
         </is>
       </c>
-      <c r="C55" s="8" t="inlineStr">
+      <c r="C55" s="7" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D55" s="8" t="inlineStr">
+      <c r="D55" s="7" t="inlineStr">
         <is>
           <t>Entrada: 08:46:18</t>
         </is>
@@ -1417,142 +1391,142 @@
     </row>
     <row r="56"/>
     <row r="57">
-      <c r="A57" s="2" t="inlineStr">
+      <c r="A57" s="3" t="inlineStr">
         <is>
           <t>TURMA: EM2102</t>
         </is>
       </c>
-      <c r="B57" s="3" t="n"/>
-      <c r="C57" s="3" t="n"/>
-      <c r="D57" s="4" t="n"/>
+      <c r="B57" s="2" t="n"/>
+      <c r="C57" s="2" t="n"/>
+      <c r="D57" s="2" t="n"/>
     </row>
     <row r="58">
-      <c r="A58" s="5" t="inlineStr">
+      <c r="A58" s="4" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B58" s="5" t="inlineStr">
+      <c r="B58" s="4" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C58" s="5" t="inlineStr">
+      <c r="C58" s="4" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D58" s="5" t="inlineStr">
+      <c r="D58" s="4" t="inlineStr">
         <is>
           <t>Acesso</t>
         </is>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="7" t="inlineStr">
+      <c r="A59" s="6" t="inlineStr">
         <is>
           <t>2025000574</t>
         </is>
       </c>
-      <c r="B59" s="7" t="inlineStr">
+      <c r="B59" s="6" t="inlineStr">
         <is>
           <t>Arthur Lopes Marino</t>
         </is>
       </c>
-      <c r="C59" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D59" s="7" t="inlineStr">
+      <c r="C59" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D59" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="7" t="inlineStr">
+      <c r="A60" s="6" t="inlineStr">
         <is>
           <t>2025000755</t>
         </is>
       </c>
-      <c r="B60" s="7" t="inlineStr">
+      <c r="B60" s="6" t="inlineStr">
         <is>
           <t>Isabela Tinoco Boechat</t>
         </is>
       </c>
-      <c r="C60" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D60" s="7" t="inlineStr">
+      <c r="C60" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D60" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="7" t="inlineStr">
+      <c r="A61" s="6" t="inlineStr">
         <is>
           <t>2025000602</t>
         </is>
       </c>
-      <c r="B61" s="7" t="inlineStr">
+      <c r="B61" s="6" t="inlineStr">
         <is>
           <t>Layla Cônçole Lage Ferreira</t>
         </is>
       </c>
-      <c r="C61" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D61" s="7" t="inlineStr">
+      <c r="C61" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D61" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="8" t="inlineStr">
+      <c r="A62" s="7" t="inlineStr">
         <is>
           <t>2025000606</t>
         </is>
       </c>
-      <c r="B62" s="8" t="inlineStr">
+      <c r="B62" s="7" t="inlineStr">
         <is>
           <t>Miguel Moraes Peixoto</t>
         </is>
       </c>
-      <c r="C62" s="8" t="inlineStr">
+      <c r="C62" s="7" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D62" s="8" t="inlineStr">
+      <c r="D62" s="7" t="inlineStr">
         <is>
           <t>Entrada: 08:49:41</t>
         </is>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="8" t="inlineStr">
+      <c r="A63" s="7" t="inlineStr">
         <is>
           <t>2025000610</t>
         </is>
       </c>
-      <c r="B63" s="8" t="inlineStr">
+      <c r="B63" s="7" t="inlineStr">
         <is>
           <t>Pablo da Silva Soares</t>
         </is>
       </c>
-      <c r="C63" s="8" t="inlineStr">
+      <c r="C63" s="7" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D63" s="8" t="inlineStr">
+      <c r="D63" s="7" t="inlineStr">
         <is>
           <t>Entrada: 08:46:27</t>
         </is>
@@ -1560,142 +1534,142 @@
     </row>
     <row r="64"/>
     <row r="65">
-      <c r="A65" s="2" t="inlineStr">
+      <c r="A65" s="3" t="inlineStr">
         <is>
           <t>TURMA: EM2201</t>
         </is>
       </c>
-      <c r="B65" s="3" t="n"/>
-      <c r="C65" s="3" t="n"/>
-      <c r="D65" s="4" t="n"/>
+      <c r="B65" s="2" t="n"/>
+      <c r="C65" s="2" t="n"/>
+      <c r="D65" s="2" t="n"/>
     </row>
     <row r="66">
-      <c r="A66" s="5" t="inlineStr">
+      <c r="A66" s="4" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B66" s="5" t="inlineStr">
+      <c r="B66" s="4" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C66" s="5" t="inlineStr">
+      <c r="C66" s="4" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D66" s="5" t="inlineStr">
+      <c r="D66" s="4" t="inlineStr">
         <is>
           <t>Acesso</t>
         </is>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="7" t="inlineStr">
+      <c r="A67" s="6" t="inlineStr">
         <is>
           <t>2024000466</t>
         </is>
       </c>
-      <c r="B67" s="7" t="inlineStr">
+      <c r="B67" s="6" t="inlineStr">
         <is>
           <t>Laura Peixoto Vieira Alves</t>
         </is>
       </c>
-      <c r="C67" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D67" s="7" t="inlineStr">
+      <c r="C67" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D67" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="8" t="inlineStr">
+      <c r="A68" s="7" t="inlineStr">
         <is>
           <t>2025000752</t>
         </is>
       </c>
-      <c r="B68" s="8" t="inlineStr">
+      <c r="B68" s="7" t="inlineStr">
         <is>
           <t>Luiza Fonseca Monteiro</t>
         </is>
       </c>
-      <c r="C68" s="8" t="inlineStr">
+      <c r="C68" s="7" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D68" s="8" t="inlineStr">
+      <c r="D68" s="7" t="inlineStr">
         <is>
           <t>Entrada: 08:08:17</t>
         </is>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="7" t="inlineStr">
+      <c r="A69" s="6" t="inlineStr">
         <is>
           <t>2024000474</t>
         </is>
       </c>
-      <c r="B69" s="7" t="inlineStr">
+      <c r="B69" s="6" t="inlineStr">
         <is>
           <t>Maria Eduarda Ramos Pedro</t>
         </is>
       </c>
-      <c r="C69" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D69" s="7" t="inlineStr">
+      <c r="C69" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D69" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="8" t="inlineStr">
+      <c r="A70" s="7" t="inlineStr">
         <is>
           <t>2024000293</t>
         </is>
       </c>
-      <c r="B70" s="8" t="inlineStr">
+      <c r="B70" s="7" t="inlineStr">
         <is>
           <t>Maria Vitória Figueira Torres</t>
         </is>
       </c>
-      <c r="C70" s="8" t="inlineStr">
+      <c r="C70" s="7" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D70" s="8" t="inlineStr">
+      <c r="D70" s="7" t="inlineStr">
         <is>
           <t>Entrada: 08:08:20</t>
         </is>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="8" t="inlineStr">
+      <c r="A71" s="7" t="inlineStr">
         <is>
           <t>2024000460</t>
         </is>
       </c>
-      <c r="B71" s="8" t="inlineStr">
+      <c r="B71" s="7" t="inlineStr">
         <is>
           <t>Welington Vioti Nascif de Mendonça Thurler</t>
         </is>
       </c>
-      <c r="C71" s="8" t="inlineStr">
+      <c r="C71" s="7" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D71" s="8" t="inlineStr">
+      <c r="D71" s="7" t="inlineStr">
         <is>
           <t>Entrada: 08:08:24</t>
         </is>
@@ -1703,98 +1677,98 @@
     </row>
     <row r="72"/>
     <row r="73">
-      <c r="A73" s="2" t="inlineStr">
+      <c r="A73" s="3" t="inlineStr">
         <is>
           <t>TURMA: EM2202</t>
         </is>
       </c>
-      <c r="B73" s="3" t="n"/>
-      <c r="C73" s="3" t="n"/>
-      <c r="D73" s="4" t="n"/>
+      <c r="B73" s="2" t="n"/>
+      <c r="C73" s="2" t="n"/>
+      <c r="D73" s="2" t="n"/>
     </row>
     <row r="74">
-      <c r="A74" s="5" t="inlineStr">
+      <c r="A74" s="4" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B74" s="5" t="inlineStr">
+      <c r="B74" s="4" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C74" s="5" t="inlineStr">
+      <c r="C74" s="4" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D74" s="5" t="inlineStr">
+      <c r="D74" s="4" t="inlineStr">
         <is>
           <t>Acesso</t>
         </is>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="8" t="inlineStr">
+      <c r="A75" s="7" t="inlineStr">
         <is>
           <t>2024000296</t>
         </is>
       </c>
-      <c r="B75" s="8" t="inlineStr">
+      <c r="B75" s="7" t="inlineStr">
         <is>
           <t>Lara Vasconcelos Souza Ferreira Lima</t>
         </is>
       </c>
-      <c r="C75" s="8" t="inlineStr">
+      <c r="C75" s="7" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D75" s="8" t="inlineStr">
+      <c r="D75" s="7" t="inlineStr">
         <is>
           <t>Entrada: 08:57:15</t>
         </is>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="7" t="inlineStr">
+      <c r="A76" s="6" t="inlineStr">
         <is>
           <t>2024000289</t>
         </is>
       </c>
-      <c r="B76" s="7" t="inlineStr">
+      <c r="B76" s="6" t="inlineStr">
         <is>
           <t>Ricardo de Almeida Nunes Pessanha</t>
         </is>
       </c>
-      <c r="C76" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D76" s="7" t="inlineStr">
+      <c r="C76" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D76" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="7" t="inlineStr">
+      <c r="A77" s="6" t="inlineStr">
         <is>
           <t>2024000279</t>
         </is>
       </c>
-      <c r="B77" s="7" t="inlineStr">
+      <c r="B77" s="6" t="inlineStr">
         <is>
           <t>Sophia Nuss Nogueira da Gama Costa Siqueira</t>
         </is>
       </c>
-      <c r="C77" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D77" s="7" t="inlineStr">
+      <c r="C77" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D77" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
@@ -1802,230 +1776,230 @@
     </row>
     <row r="78"/>
     <row r="79">
-      <c r="A79" s="2" t="inlineStr">
+      <c r="A79" s="3" t="inlineStr">
         <is>
           <t>TURMA: EM2301</t>
         </is>
       </c>
-      <c r="B79" s="3" t="n"/>
-      <c r="C79" s="3" t="n"/>
-      <c r="D79" s="4" t="n"/>
+      <c r="B79" s="2" t="n"/>
+      <c r="C79" s="2" t="n"/>
+      <c r="D79" s="2" t="n"/>
     </row>
     <row r="80">
-      <c r="A80" s="5" t="inlineStr">
+      <c r="A80" s="4" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B80" s="5" t="inlineStr">
+      <c r="B80" s="4" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C80" s="5" t="inlineStr">
+      <c r="C80" s="4" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D80" s="5" t="inlineStr">
+      <c r="D80" s="4" t="inlineStr">
         <is>
           <t>Acesso</t>
         </is>
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="7" t="inlineStr">
+      <c r="A81" s="6" t="inlineStr">
         <is>
           <t>2023000031</t>
         </is>
       </c>
-      <c r="B81" s="7" t="inlineStr">
+      <c r="B81" s="6" t="inlineStr">
         <is>
           <t>Antonella Tavares Soares</t>
         </is>
       </c>
-      <c r="C81" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D81" s="7" t="inlineStr">
+      <c r="C81" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D81" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="7" t="inlineStr">
+      <c r="A82" s="6" t="inlineStr">
         <is>
           <t>2023000174</t>
         </is>
       </c>
-      <c r="B82" s="7" t="inlineStr">
+      <c r="B82" s="6" t="inlineStr">
         <is>
           <t>Bruno de Oliveira Vieira</t>
         </is>
       </c>
-      <c r="C82" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D82" s="7" t="inlineStr">
+      <c r="C82" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D82" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="7" t="inlineStr">
+      <c r="A83" s="6" t="inlineStr">
         <is>
           <t>2023000035</t>
         </is>
       </c>
-      <c r="B83" s="7" t="inlineStr">
+      <c r="B83" s="6" t="inlineStr">
         <is>
           <t>Davi Meirelles de Freitas</t>
         </is>
       </c>
-      <c r="C83" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D83" s="7" t="inlineStr">
+      <c r="C83" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D83" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="7" t="inlineStr">
+      <c r="A84" s="6" t="inlineStr">
         <is>
           <t>2023000155</t>
         </is>
       </c>
-      <c r="B84" s="7" t="inlineStr">
+      <c r="B84" s="6" t="inlineStr">
         <is>
           <t>Felipe Evaristo da Silva Marcolongo</t>
         </is>
       </c>
-      <c r="C84" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D84" s="7" t="inlineStr">
+      <c r="C84" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D84" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="6" t="inlineStr">
+      <c r="A85" s="5" t="inlineStr">
         <is>
           <t>2023000052</t>
         </is>
       </c>
-      <c r="B85" s="6" t="inlineStr">
+      <c r="B85" s="5" t="inlineStr">
         <is>
           <t>João Pedro Mançano Bastos da Cruz</t>
         </is>
       </c>
-      <c r="C85" s="6" t="inlineStr">
+      <c r="C85" s="5" t="inlineStr">
         <is>
           <t>SAIU CEDO</t>
         </is>
       </c>
-      <c r="D85" s="6" t="inlineStr">
+      <c r="D85" s="5" t="inlineStr">
         <is>
           <t>Saída: 10:44:57</t>
         </is>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="7" t="inlineStr">
+      <c r="A86" s="6" t="inlineStr">
         <is>
           <t>2023000056</t>
         </is>
       </c>
-      <c r="B86" s="7" t="inlineStr">
+      <c r="B86" s="6" t="inlineStr">
         <is>
           <t>Leon Fontoura Gonçalves</t>
         </is>
       </c>
-      <c r="C86" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D86" s="7" t="inlineStr">
+      <c r="C86" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D86" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="6" t="inlineStr">
+      <c r="A87" s="5" t="inlineStr">
         <is>
           <t>2023000060</t>
         </is>
       </c>
-      <c r="B87" s="6" t="inlineStr">
+      <c r="B87" s="5" t="inlineStr">
         <is>
           <t>Luíza Arantes Rangel Muniz</t>
         </is>
       </c>
-      <c r="C87" s="6" t="inlineStr">
+      <c r="C87" s="5" t="inlineStr">
         <is>
           <t>SAIU CEDO</t>
         </is>
       </c>
-      <c r="D87" s="6" t="inlineStr">
+      <c r="D87" s="5" t="inlineStr">
         <is>
           <t>Saída: 10:44:52</t>
         </is>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="7" t="inlineStr">
+      <c r="A88" s="6" t="inlineStr">
         <is>
           <t>2024000504</t>
         </is>
       </c>
-      <c r="B88" s="7" t="inlineStr">
+      <c r="B88" s="6" t="inlineStr">
         <is>
           <t>Murilo Kunze Soares</t>
         </is>
       </c>
-      <c r="C88" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D88" s="7" t="inlineStr">
+      <c r="C88" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D88" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="7" t="inlineStr">
+      <c r="A89" s="6" t="inlineStr">
         <is>
           <t>2023000202</t>
         </is>
       </c>
-      <c r="B89" s="7" t="inlineStr">
+      <c r="B89" s="6" t="inlineStr">
         <is>
           <t>Patrícia Resende Rodrigues da Silva</t>
         </is>
       </c>
-      <c r="C89" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D89" s="7" t="inlineStr">
+      <c r="C89" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D89" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
@@ -2033,472 +2007,472 @@
     </row>
     <row r="90"/>
     <row r="91">
-      <c r="A91" s="2" t="inlineStr">
+      <c r="A91" s="3" t="inlineStr">
         <is>
           <t>TURMA: EM2302</t>
         </is>
       </c>
-      <c r="B91" s="3" t="n"/>
-      <c r="C91" s="3" t="n"/>
-      <c r="D91" s="4" t="n"/>
+      <c r="B91" s="2" t="n"/>
+      <c r="C91" s="2" t="n"/>
+      <c r="D91" s="2" t="n"/>
     </row>
     <row r="92">
-      <c r="A92" s="5" t="inlineStr">
+      <c r="A92" s="4" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B92" s="5" t="inlineStr">
+      <c r="B92" s="4" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C92" s="5" t="inlineStr">
+      <c r="C92" s="4" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D92" s="5" t="inlineStr">
+      <c r="D92" s="4" t="inlineStr">
         <is>
           <t>Acesso</t>
         </is>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="7" t="inlineStr">
+      <c r="A93" s="6" t="inlineStr">
         <is>
           <t>2023000028</t>
         </is>
       </c>
-      <c r="B93" s="7" t="inlineStr">
+      <c r="B93" s="6" t="inlineStr">
         <is>
           <t>Alice Pereira Baptista</t>
         </is>
       </c>
-      <c r="C93" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D93" s="7" t="inlineStr">
+      <c r="C93" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D93" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="7" t="inlineStr">
+      <c r="A94" s="6" t="inlineStr">
         <is>
           <t>2023000168</t>
         </is>
       </c>
-      <c r="B94" s="7" t="inlineStr">
+      <c r="B94" s="6" t="inlineStr">
         <is>
           <t>Ana Luísa Petterman Galito</t>
         </is>
       </c>
-      <c r="C94" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D94" s="7" t="inlineStr">
+      <c r="C94" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D94" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="7" t="inlineStr">
+      <c r="A95" s="6" t="inlineStr">
         <is>
           <t>2023000218</t>
         </is>
       </c>
-      <c r="B95" s="7" t="inlineStr">
+      <c r="B95" s="6" t="inlineStr">
         <is>
           <t>Arthur Ponciano Frontelmo Rangel</t>
         </is>
       </c>
-      <c r="C95" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D95" s="7" t="inlineStr">
+      <c r="C95" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D95" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="7" t="inlineStr">
+      <c r="A96" s="6" t="inlineStr">
         <is>
           <t>2023000033</t>
         </is>
       </c>
-      <c r="B96" s="7" t="inlineStr">
+      <c r="B96" s="6" t="inlineStr">
         <is>
           <t>Carolina Rodrigues de Britto</t>
         </is>
       </c>
-      <c r="C96" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D96" s="7" t="inlineStr">
+      <c r="C96" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D96" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="7" t="inlineStr">
+      <c r="A97" s="6" t="inlineStr">
         <is>
           <t>2023000039</t>
         </is>
       </c>
-      <c r="B97" s="7" t="inlineStr">
+      <c r="B97" s="6" t="inlineStr">
         <is>
           <t>Diana Alves Fortuna Pussiareli</t>
         </is>
       </c>
-      <c r="C97" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D97" s="7" t="inlineStr">
+      <c r="C97" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D97" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="7" t="inlineStr">
+      <c r="A98" s="6" t="inlineStr">
         <is>
           <t>2023000145</t>
         </is>
       </c>
-      <c r="B98" s="7" t="inlineStr">
+      <c r="B98" s="6" t="inlineStr">
         <is>
           <t>Décio Macedo Netto</t>
         </is>
       </c>
-      <c r="C98" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D98" s="7" t="inlineStr">
+      <c r="C98" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D98" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="7" t="inlineStr">
+      <c r="A99" s="6" t="inlineStr">
         <is>
           <t>2025000742</t>
         </is>
       </c>
-      <c r="B99" s="7" t="inlineStr">
+      <c r="B99" s="6" t="inlineStr">
         <is>
           <t>Gabriel Guilherme Ribeiro</t>
         </is>
       </c>
-      <c r="C99" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D99" s="7" t="inlineStr">
+      <c r="C99" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D99" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="7" t="inlineStr">
+      <c r="A100" s="6" t="inlineStr">
         <is>
           <t>2023000046</t>
         </is>
       </c>
-      <c r="B100" s="7" t="inlineStr">
+      <c r="B100" s="6" t="inlineStr">
         <is>
           <t>Guilherme de Oliveira Avelino</t>
         </is>
       </c>
-      <c r="C100" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D100" s="7" t="inlineStr">
+      <c r="C100" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D100" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="7" t="inlineStr">
+      <c r="A101" s="6" t="inlineStr">
         <is>
           <t>2023000043</t>
         </is>
       </c>
-      <c r="B101" s="7" t="inlineStr">
+      <c r="B101" s="6" t="inlineStr">
         <is>
           <t>Gustavo Martins Moura Cruz</t>
         </is>
       </c>
-      <c r="C101" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D101" s="7" t="inlineStr">
+      <c r="C101" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D101" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="6" t="inlineStr">
+      <c r="A102" s="5" t="inlineStr">
         <is>
           <t>2023000048</t>
         </is>
       </c>
-      <c r="B102" s="6" t="inlineStr">
+      <c r="B102" s="5" t="inlineStr">
         <is>
           <t>Isaac Costa da Silva Venturi</t>
         </is>
       </c>
-      <c r="C102" s="6" t="inlineStr">
+      <c r="C102" s="5" t="inlineStr">
         <is>
           <t>SAIU CEDO</t>
         </is>
       </c>
-      <c r="D102" s="6" t="inlineStr">
+      <c r="D102" s="5" t="inlineStr">
         <is>
           <t>Saída: 10:45:38</t>
         </is>
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="7" t="inlineStr">
+      <c r="A103" s="6" t="inlineStr">
         <is>
           <t>2023000049</t>
         </is>
       </c>
-      <c r="B103" s="7" t="inlineStr">
+      <c r="B103" s="6" t="inlineStr">
         <is>
           <t>Isabela Poeys Rocha</t>
         </is>
       </c>
-      <c r="C103" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D103" s="7" t="inlineStr">
+      <c r="C103" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D103" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="6" t="inlineStr">
+      <c r="A104" s="5" t="inlineStr">
         <is>
           <t>2023000050</t>
         </is>
       </c>
-      <c r="B104" s="6" t="inlineStr">
+      <c r="B104" s="5" t="inlineStr">
         <is>
           <t>João Lucas Ximenes Diniz</t>
         </is>
       </c>
-      <c r="C104" s="6" t="inlineStr">
+      <c r="C104" s="5" t="inlineStr">
         <is>
           <t>SAIU CEDO</t>
         </is>
       </c>
-      <c r="D104" s="6" t="inlineStr">
+      <c r="D104" s="5" t="inlineStr">
         <is>
           <t>Saída: 10:45:31</t>
         </is>
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="8" t="inlineStr">
+      <c r="A105" s="7" t="inlineStr">
         <is>
           <t>2023000054</t>
         </is>
       </c>
-      <c r="B105" s="8" t="inlineStr">
+      <c r="B105" s="7" t="inlineStr">
         <is>
           <t>Júlia Montovani Patrício</t>
         </is>
       </c>
-      <c r="C105" s="8" t="inlineStr">
+      <c r="C105" s="7" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D105" s="8" t="inlineStr">
+      <c r="D105" s="7" t="inlineStr">
         <is>
           <t>Entrada: 08:44:11</t>
         </is>
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="8" t="inlineStr">
+      <c r="A106" s="7" t="inlineStr">
         <is>
           <t>2023000166</t>
         </is>
       </c>
-      <c r="B106" s="8" t="inlineStr">
+      <c r="B106" s="7" t="inlineStr">
         <is>
           <t>Lícia Tinoco Dias</t>
         </is>
       </c>
-      <c r="C106" s="8" t="inlineStr">
+      <c r="C106" s="7" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D106" s="8" t="inlineStr">
+      <c r="D106" s="7" t="inlineStr">
         <is>
           <t>Entrada: 08:59:16</t>
         </is>
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="7" t="inlineStr">
+      <c r="A107" s="6" t="inlineStr">
         <is>
           <t>2023000006</t>
         </is>
       </c>
-      <c r="B107" s="7" t="inlineStr">
+      <c r="B107" s="6" t="inlineStr">
         <is>
           <t>Pedro da Silva Pereira Ferreira</t>
         </is>
       </c>
-      <c r="C107" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D107" s="7" t="inlineStr">
+      <c r="C107" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D107" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="6" t="inlineStr">
+      <c r="A108" s="5" t="inlineStr">
         <is>
           <t>2023000074</t>
         </is>
       </c>
-      <c r="B108" s="6" t="inlineStr">
+      <c r="B108" s="5" t="inlineStr">
         <is>
           <t>Rafael Tinoco Novaes Lannes Santucci</t>
         </is>
       </c>
-      <c r="C108" s="6" t="inlineStr">
+      <c r="C108" s="5" t="inlineStr">
         <is>
           <t>SAIU CEDO</t>
         </is>
       </c>
-      <c r="D108" s="6" t="inlineStr">
+      <c r="D108" s="5" t="inlineStr">
         <is>
           <t>Saída: 10:43:59</t>
         </is>
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="7" t="inlineStr">
+      <c r="A109" s="6" t="inlineStr">
         <is>
           <t>2023000075</t>
         </is>
       </c>
-      <c r="B109" s="7" t="inlineStr">
+      <c r="B109" s="6" t="inlineStr">
         <is>
           <t>Raphaela Crespo Bastos</t>
         </is>
       </c>
-      <c r="C109" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D109" s="7" t="inlineStr">
+      <c r="C109" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D109" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="6" t="inlineStr">
+      <c r="A110" s="5" t="inlineStr">
         <is>
           <t>2023000076</t>
         </is>
       </c>
-      <c r="B110" s="6" t="inlineStr">
+      <c r="B110" s="5" t="inlineStr">
         <is>
           <t>Ray da Silva Martins Bizarro</t>
         </is>
       </c>
-      <c r="C110" s="6" t="inlineStr">
+      <c r="C110" s="5" t="inlineStr">
         <is>
           <t>SAIU CEDO</t>
         </is>
       </c>
-      <c r="D110" s="6" t="inlineStr">
+      <c r="D110" s="5" t="inlineStr">
         <is>
           <t>Saída: 10:44:23</t>
         </is>
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="8" t="inlineStr">
+      <c r="A111" s="7" t="inlineStr">
         <is>
           <t>2025000758</t>
         </is>
       </c>
-      <c r="B111" s="8" t="inlineStr">
+      <c r="B111" s="7" t="inlineStr">
         <is>
           <t>Víctor Machado Perusso de Souza</t>
         </is>
       </c>
-      <c r="C111" s="8" t="inlineStr">
+      <c r="C111" s="7" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D111" s="8" t="inlineStr">
+      <c r="D111" s="7" t="inlineStr">
         <is>
           <t>Entrada: 10:45:04</t>
         </is>
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="7" t="inlineStr">
+      <c r="A112" s="6" t="inlineStr">
         <is>
           <t>2023000027</t>
         </is>
       </c>
-      <c r="B112" s="7" t="inlineStr">
+      <c r="B112" s="6" t="inlineStr">
         <is>
           <t>Ágata Priscila André Tarouquela</t>
         </is>
       </c>
-      <c r="C112" s="7" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D112" s="7" t="inlineStr">
+      <c r="C112" s="6" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D112" s="6" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>

</xml_diff>